<commit_message>
caorimetry : GUI regression tests : EMF
</commit_message>
<xml_diff>
--- a/tests/data.gui/test/emf/dsp.1/kev.emf.constants.data.xlsx
+++ b/tests/data.gui/test/emf/dsp.1/kev.emf.constants.data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve">H</t>
   </si>
@@ -273,10 +273,13 @@
     <t xml:space="preserve">4.971923828125</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0185485041910094</t>
+    <t xml:space="preserve">0.0185485041909776</t>
   </si>
   <si>
     <t xml:space="preserve">Adj. R^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.981564</t>
   </si>
 </sst>
 </file>
@@ -708,8 +711,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.981564101396708</v>
+      <c r="A2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1100,16 +1103,16 @@
         <v>0.00032745462855956</v>
       </c>
       <c r="C2" t="n">
-        <v>2.80095503833757e-16</v>
+        <v>0.000000000000000280095503833757</v>
       </c>
       <c r="D2" t="n">
         <v>0.00984254080982287</v>
       </c>
       <c r="E2" t="n">
-        <v>4.56161755220153e-09</v>
+        <v>0.00000000456161755220153</v>
       </c>
       <c r="F2" t="n">
-        <v>6.81300017301869e-06</v>
+        <v>0.00000681300017301864</v>
       </c>
     </row>
     <row r="3">
@@ -1120,33 +1123,33 @@
         <v>0.000694492143695651</v>
       </c>
       <c r="C3" t="n">
-        <v>4.99889027881563e-14</v>
+        <v>0.0000000000000499889027881561</v>
       </c>
       <c r="D3" t="n">
         <v>0.00943548645234059</v>
       </c>
       <c r="E3" t="n">
-        <v>2.14039637703211e-08</v>
+        <v>0.0000000214039637703211</v>
       </c>
       <c r="F3" t="n">
-        <v>0.000549600013251644</v>
+        <v>0.00054960001325164</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7.48952076072689e-05</v>
+        <v>0.000074895207607269</v>
       </c>
       <c r="B4" t="n">
         <v>0.00125674529994241</v>
       </c>
       <c r="C4" t="n">
-        <v>2.08047957926759e-13</v>
+        <v>0.000000000000208047957926759</v>
       </c>
       <c r="D4" t="n">
         <v>0.0088231797463292</v>
       </c>
       <c r="E4" t="n">
-        <v>7.49537284068671e-08</v>
+        <v>0.0000000749537284068668</v>
       </c>
       <c r="F4" t="n">
         <v>0.00118200002666069</v>
@@ -1154,19 +1157,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.47041594707056e-05</v>
+        <v>0.0000447041594707056</v>
       </c>
       <c r="B5" t="n">
         <v>0.00193231800480312</v>
       </c>
       <c r="C5" t="n">
-        <v>5.56742102803982e-13</v>
+        <v>0.000000000000556742102803984</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00809748891814147</v>
+        <v>0.00809748891814144</v>
       </c>
       <c r="E5" t="n">
-        <v>1.930770554201e-07</v>
+        <v>0.0000001930770554201</v>
       </c>
       <c r="F5" t="n">
         <v>0.00188800003973887</v>
@@ -1174,122 +1177,122 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.29753781391267e-05</v>
+        <v>0.0000329753781391267</v>
       </c>
       <c r="B6" t="n">
         <v>0.00244131397769643</v>
       </c>
       <c r="C6" t="n">
-        <v>9.6304598320478e-13</v>
+        <v>0.000000000000963045983206316</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00754635532256376</v>
+        <v>0.00754635532256373</v>
       </c>
       <c r="E6" t="n">
-        <v>3.3069973982554e-07</v>
+        <v>0.00000033069973982554</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00240900004776922</v>
+        <v>0.00240900004777305</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.49047778656104e-05</v>
+        <v>0.0000249047778656105</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00298283479417156</v>
+        <v>0.00298283479417155</v>
       </c>
       <c r="C7" t="n">
-        <v>1.56625438830958e-12</v>
+        <v>0.00000000000156625438830669</v>
       </c>
       <c r="D7" t="n">
         <v>0.00696363021476453</v>
       </c>
       <c r="E7" t="n">
-        <v>5.34991063900732e-07</v>
+        <v>0.00000053499106390073</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00295900005522472</v>
+        <v>0.00295900005521927</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.25627165721912e-05</v>
+        <v>0.0000125627165721912</v>
       </c>
       <c r="B8" t="n">
         <v>0.00451335314998711</v>
       </c>
       <c r="C8" t="n">
-        <v>4.72622971950048e-12</v>
+        <v>0.00000000000472622971951294</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00531504206908348</v>
+        <v>0.00531504206908346</v>
       </c>
       <c r="E8" t="n">
-        <v>1.60478092942479e-06</v>
+        <v>0.00000160478092942479</v>
       </c>
       <c r="F8" t="n">
-        <v>0.004504000069529</v>
+        <v>0.00450400006954087</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9.69699446366105e-06</v>
+        <v>0.00000969699446366105</v>
       </c>
       <c r="B9" t="n">
         <v>0.00512397635747019</v>
       </c>
       <c r="C9" t="n">
-        <v>6.9590184520488e-12</v>
+        <v>0.00000000000695901845201884</v>
       </c>
       <c r="D9" t="n">
         <v>0.00465766332751259</v>
       </c>
       <c r="E9" t="n">
-        <v>2.36031501722367e-06</v>
+        <v>0.00000236031501722367</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00511900007246917</v>
+        <v>0.00511900007244713</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7.90192933202366e-06</v>
+        <v>0.00000790192933202366</v>
       </c>
       <c r="B10" t="n">
         <v>0.0055975734801322</v>
       </c>
       <c r="C10" t="n">
-        <v>9.33565018823056e-12</v>
+        <v>0.00000000000933565018824764</v>
       </c>
       <c r="D10" t="n">
         <v>0.00414626229993571</v>
       </c>
       <c r="E10" t="n">
-        <v>3.16421993208853e-06</v>
+        <v>0.00000316421993208853</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00559600007329945</v>
+        <v>0.00559600007330967</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6.23532677520115e-06</v>
+        <v>0.00000623532677520116</v>
       </c>
       <c r="B11" t="n">
         <v>0.00612346191648993</v>
       </c>
       <c r="C11" t="n">
-        <v>1.29514316852232e-11</v>
+        <v>0.0000000000129514316851118</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00357915138484314</v>
+        <v>0.00357915138484315</v>
       </c>
       <c r="E11" t="n">
-        <v>4.38669866691808e-06</v>
+        <v>0.00000438669866691807</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0061260000728307</v>
+        <v>0.00612600007277803</v>
       </c>
     </row>
   </sheetData>
@@ -1364,10 +1367,10 @@
         <v>107.606462597853</v>
       </c>
       <c r="G2" t="n">
-        <v>99.0743324834217</v>
+        <v>99.0743324834216</v>
       </c>
       <c r="H2" t="n">
-        <v>91.2040093341404</v>
+        <v>91.2040093341405</v>
       </c>
       <c r="I2" t="n">
         <v>72.0168347467973</v>
@@ -1390,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.850557133161942</v>
+        <v>-0.850557133161971</v>
       </c>
       <c r="D3" t="n">
         <v>-1.41466272446311</v>
@@ -1399,13 +1402,13 @@
         <v>-1.22524789010117</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.09353740214674</v>
+        <v>-3.09353740214679</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.32566751657833</v>
+        <v>-3.32566751657839</v>
       </c>
       <c r="H3" t="n">
-        <v>-2.99599066585958</v>
+        <v>-2.99599066585952</v>
       </c>
       <c r="I3" t="n">
         <v>-0.183165253202702</v>
@@ -1492,10 +1495,10 @@
         <v>107.606462597853</v>
       </c>
       <c r="G2" t="n">
-        <v>99.0743324834217</v>
+        <v>99.0743324834216</v>
       </c>
       <c r="H2" t="n">
-        <v>91.2040093341404</v>
+        <v>91.2040093341405</v>
       </c>
       <c r="I2" t="n">
         <v>72.0168347467973</v>
@@ -1518,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00519582854711022</v>
+        <v>-0.00519582854711039</v>
       </c>
       <c r="D3" t="n">
         <v>-0.00996241355255714</v>
@@ -1527,13 +1530,13 @@
         <v>-0.00993712806245882</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0279452339850654</v>
+        <v>-0.0279452339850659</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0324772218415853</v>
+        <v>-0.0324772218415859</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0318045718244117</v>
+        <v>-0.0318045718244111</v>
       </c>
       <c r="I3" t="n">
         <v>-0.00253691486430335</v>

</xml_diff>